<commit_message>
-1 as contsVerNo, 변경
</commit_message>
<xml_diff>
--- a/src/main/resources/database/메뉴별 라우팅구조(CMS_표기).xlsx
+++ b/src/main/resources/database/메뉴별 라우팅구조(CMS_표기).xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\drugsafe\doc\UI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drugsafe\sources\to_be\pp-be\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BADB39-86AB-4C83-A023-2F2BBE8185D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2CF5B5-71EC-43C2-9F26-48A83DAA0854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F936E8C6-739C-498F-B507-DC33B8FB3111}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F936E8C6-739C-498F-B507-DC33B8FB3111}"/>
   </bookViews>
   <sheets>
     <sheet name="MENU" sheetId="1" r:id="rId1"/>
     <sheet name="CMS_URL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MENU!$A$1:$L$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MENU!$A$1:$M$96</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="299">
   <si>
     <t>ko</t>
   </si>
@@ -542,10 +542,6 @@
     <t>01 &gt; 35</t>
   </si>
   <si>
-    <t>화면내 탭(상세) 업무</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">  /maintask/relief</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -630,10 +626,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">  /safe/ReliefNews.tsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">    /maintask/relief/ReliefNews.tsx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1073,6 +1065,87 @@
   </si>
   <si>
     <t>conts_sn 값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판_ID
+(bbs_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_COM_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_COM_002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_GAL_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_VDO_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_COM_005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_DUR_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_FAQ_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_PRESS_001</t>
+  </si>
+  <si>
+    <t>BBS_LETTER_001</t>
+  </si>
+  <si>
+    <t>BBS_LEAFLET_001</t>
+  </si>
+  <si>
+    <t>BBS_ABOUT_NEWS_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_REAL_NAME_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_EXPS_DETAILS_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_BIZ_TRIPS_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_RELIEF_NEWS_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  /safe/DrugNews.tsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_DRUG_NEWS_001</t>
+  </si>
+  <si>
+    <t>BBS_ADVERSE_GUD_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBS_ADVERSE_DATA_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화면내 탭 업무</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1080,7 +1153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1145,14 +1218,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="26"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -1174,6 +1239,15 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1311,19 +1385,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1645,27 +1719,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F1065D-2337-4AD4-BE05-642580AA564F}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="3"/>
-    <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="8.09765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.296875" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" customWidth="1"/>
     <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.875" customWidth="1"/>
-    <col min="6" max="6" width="14.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.25" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.75" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.09765625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.19921875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.59765625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.69921875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.09765625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33">
+    <row r="1" spans="1:13" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>67</v>
       </c>
@@ -1673,13 +1748,13 @@
         <v>68</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>142</v>
+        <v>298</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>69</v>
@@ -1693,17 +1768,20 @@
       <c r="I1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1725,15 +1803,16 @@
       <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="J2" s="5"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1757,15 +1836,16 @@
       <c r="I3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1789,15 +1869,16 @@
       <c r="I4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="J4" s="5"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1805,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>88</v>
@@ -1823,17 +1904,18 @@
       <c r="I5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="5"/>
+      <c r="K5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1841,7 +1923,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>89</v>
@@ -1859,17 +1941,18 @@
       <c r="I6" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="J6" s="5"/>
+      <c r="K6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1893,15 +1976,16 @@
       <c r="I7" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2">
-        <v>2</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="J7" s="5"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1909,7 +1993,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>121</v>
@@ -1927,15 +2011,16 @@
       <c r="I8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="J8" s="5"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1943,7 +2028,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>122</v>
@@ -1961,15 +2046,16 @@
       <c r="I9" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="2">
-        <v>2</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="J9" s="5"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1977,10 +2063,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2">
@@ -1995,17 +2081,18 @@
       <c r="I10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="J10" s="5"/>
+      <c r="K10" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="L10" s="2">
         <v>3</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2013,10 +2100,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2">
@@ -2031,15 +2118,18 @@
       <c r="I11" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="2">
+      <c r="J11" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2">
         <v>4</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2047,10 +2137,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2">
@@ -2065,15 +2155,18 @@
       <c r="I12" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="2">
+      <c r="J12" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2">
         <v>5</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2097,15 +2190,16 @@
       <c r="I13" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="2">
-        <v>2</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="J13" s="5"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2113,10 +2207,10 @@
         <v>83</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="2">
@@ -2131,17 +2225,18 @@
       <c r="I14" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="J14" s="5"/>
+      <c r="K14" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2149,7 +2244,7 @@
         <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>123</v>
@@ -2167,15 +2262,16 @@
       <c r="I15" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="2">
-        <v>2</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="J15" s="5"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2">
+        <v>2</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2199,15 +2295,16 @@
       <c r="I16" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="2">
+      <c r="J16" s="5"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2">
         <v>3</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2215,10 +2312,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2">
@@ -2233,17 +2330,18 @@
       <c r="I17" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="J17" s="5"/>
+      <c r="K17" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2251,10 +2349,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="2">
@@ -2269,17 +2367,18 @@
       <c r="I18" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K18" s="2">
-        <v>2</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="J18" s="5"/>
+      <c r="K18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L18" s="2">
+        <v>2</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2287,10 +2386,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="2">
@@ -2305,17 +2404,18 @@
       <c r="I19" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="K19" s="2">
+      <c r="J19" s="5"/>
+      <c r="K19" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L19" s="2">
         <v>3</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2339,15 +2439,16 @@
       <c r="I20" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="2">
+      <c r="J20" s="5"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2">
         <v>4</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2355,10 +2456,10 @@
         <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="2">
@@ -2373,23 +2474,24 @@
       <c r="I21" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="J21" s="5"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>120</v>
@@ -2407,15 +2509,16 @@
       <c r="I22" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="2">
-        <v>2</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="J22" s="5"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2">
+        <v>2</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2439,15 +2542,16 @@
       <c r="I23" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="2">
+      <c r="J23" s="5"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="2">
         <v>5</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2455,10 +2559,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="2">
@@ -2473,17 +2577,18 @@
       <c r="I24" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" s="2" t="s">
+      <c r="J24" s="5"/>
+      <c r="K24" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2491,10 +2596,10 @@
         <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="2">
@@ -2509,15 +2614,16 @@
       <c r="I25" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="2">
-        <v>2</v>
-      </c>
-      <c r="L25" s="2" t="s">
+      <c r="J25" s="5"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2">
+        <v>2</v>
+      </c>
+      <c r="M25" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2529,11 +2635,12 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="J26" s="8"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2545,11 +2652,12 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="J27" s="8"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2561,11 +2669,12 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="J28" s="8"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -2577,11 +2686,12 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="J29" s="8"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -2593,11 +2703,12 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="J30" s="8"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -2609,11 +2720,12 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="J31" s="8"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -2625,11 +2737,12 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="J32" s="8"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -2641,11 +2754,12 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" s="16" customFormat="1">
+      <c r="J33" s="8"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="12">
         <v>25</v>
       </c>
@@ -2653,10 +2767,10 @@
         <v>77</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="12">
@@ -2671,15 +2785,16 @@
       <c r="I34" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="J34" s="11"/>
-      <c r="K34" s="12">
+      <c r="J34" s="15"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12">
         <v>3</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="16" customFormat="1">
+      <c r="M34" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="12"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -2691,11 +2806,12 @@
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="15"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" s="16" customFormat="1">
+      <c r="J35" s="15"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="12"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -2707,11 +2823,12 @@
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12" s="16" customFormat="1">
+      <c r="J36" s="15"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="12"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -2723,11 +2840,12 @@
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="15"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" s="16" customFormat="1">
+      <c r="J37" s="15"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="12"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -2739,11 +2857,12 @@
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
       <c r="I38" s="15"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12" s="16" customFormat="1">
+      <c r="J38" s="15"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -2755,11 +2874,12 @@
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="15"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:12" s="16" customFormat="1">
+      <c r="J39" s="15"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="12"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -2771,11 +2891,12 @@
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="15"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" s="16" customFormat="1">
+      <c r="J40" s="15"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -2787,11 +2908,12 @@
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="15"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:12" s="16" customFormat="1">
+      <c r="J41" s="15"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="12"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -2803,11 +2925,12 @@
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
       <c r="I42" s="15"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="J42" s="15"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
         <v>26</v>
       </c>
@@ -2815,10 +2938,10 @@
         <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="2">
@@ -2833,15 +2956,16 @@
       <c r="I43" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J43" s="1"/>
-      <c r="K43" s="2">
+      <c r="J43" s="5"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="2">
         <v>4</v>
       </c>
-      <c r="L43" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -2853,11 +2977,12 @@
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="14"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="J44" s="14"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -2869,11 +2994,12 @@
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
       <c r="I45" s="14"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="J45" s="14"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -2885,11 +3011,12 @@
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
       <c r="I46" s="14"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="2"/>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="J46" s="14"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2901,11 +3028,12 @@
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
       <c r="I47" s="14"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="J47" s="14"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2917,11 +3045,12 @@
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="14"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="J48" s="14"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" s="2">
         <v>27</v>
       </c>
@@ -2929,7 +3058,7 @@
         <v>128</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>130</v>
@@ -2947,15 +3076,18 @@
       <c r="I49" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="2">
+      <c r="J49" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="K49" s="1"/>
+      <c r="L49" s="2">
         <v>5</v>
       </c>
-      <c r="L49" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" s="2">
         <v>28</v>
       </c>
@@ -2963,10 +3095,10 @@
         <v>129</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="2">
@@ -2981,15 +3113,16 @@
       <c r="I50" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="J50" s="1"/>
-      <c r="K50" s="2">
+      <c r="J50" s="5"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="2">
         <v>6</v>
       </c>
-      <c r="L50" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" s="2">
         <v>29</v>
       </c>
@@ -2998,7 +3131,7 @@
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="2">
@@ -3013,15 +3146,16 @@
       <c r="I51" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J51" s="1"/>
-      <c r="K51" s="2">
+      <c r="J51" s="5"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="2">
         <v>6</v>
       </c>
-      <c r="L51" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" s="2">
         <v>30</v>
       </c>
@@ -3029,10 +3163,10 @@
         <v>31</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="2">
@@ -3047,17 +3181,18 @@
       <c r="I52" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="K52" s="2">
-        <v>1</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="J52" s="5"/>
+      <c r="K52" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="L52" s="2">
+        <v>1</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" s="2">
         <v>31</v>
       </c>
@@ -3065,10 +3200,10 @@
         <v>32</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="2">
@@ -3083,17 +3218,18 @@
       <c r="I53" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="K53" s="2">
-        <v>2</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="J53" s="5"/>
+      <c r="K53" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L53" s="2">
+        <v>2</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A54" s="2">
         <v>32</v>
       </c>
@@ -3101,10 +3237,10 @@
         <v>133</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="2">
@@ -3119,15 +3255,18 @@
       <c r="I54" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="J54" s="1"/>
-      <c r="K54" s="2">
+      <c r="J54" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="K54" s="1"/>
+      <c r="L54" s="2">
         <v>3</v>
       </c>
-      <c r="L54" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" s="2">
         <v>33</v>
       </c>
@@ -3135,7 +3274,7 @@
         <v>33</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>134</v>
@@ -3153,15 +3292,16 @@
       <c r="I55" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="J55" s="1"/>
-      <c r="K55" s="2">
+      <c r="J55" s="5"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="2">
         <v>4</v>
       </c>
-      <c r="L55" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
         <v>34</v>
       </c>
@@ -3169,10 +3309,10 @@
         <v>49</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="2">
@@ -3187,15 +3327,16 @@
       <c r="I56" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J56" s="1"/>
-      <c r="K56" s="2">
+      <c r="J56" s="5"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="2">
         <v>7</v>
       </c>
-      <c r="L56" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" s="2">
         <v>35</v>
       </c>
@@ -3203,10 +3344,10 @@
         <v>50</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>160</v>
+        <v>294</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="2">
@@ -3221,15 +3362,18 @@
       <c r="I57" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J57" s="1"/>
-      <c r="K57" s="2">
+      <c r="J57" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="K57" s="1"/>
+      <c r="L57" s="2">
         <v>8</v>
       </c>
-      <c r="L57" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" s="2">
         <v>36</v>
       </c>
@@ -3238,7 +3382,7 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="2"/>
@@ -3251,15 +3395,16 @@
       <c r="I58" s="5">
         <v>36</v>
       </c>
-      <c r="J58" s="1"/>
-      <c r="K58" s="2">
-        <v>2</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="J58" s="5"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="2">
+        <v>2</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" s="2">
         <v>37</v>
       </c>
@@ -3268,7 +3413,7 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="2">
@@ -3281,17 +3426,18 @@
         <v>36</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="J59" s="1"/>
-      <c r="K59" s="2">
-        <v>1</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+        <v>147</v>
+      </c>
+      <c r="J59" s="5"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="2">
+        <v>1</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" s="2">
         <v>38</v>
       </c>
@@ -3299,10 +3445,10 @@
         <v>37</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="2">
@@ -3315,19 +3461,20 @@
         <v>36</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="K60" s="2">
-        <v>1</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>148</v>
+      </c>
+      <c r="J60" s="5"/>
+      <c r="K60" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="L60" s="2">
+        <v>1</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" s="2">
         <v>39</v>
       </c>
@@ -3335,10 +3482,10 @@
         <v>38</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="2">
@@ -3351,17 +3498,18 @@
         <v>36</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J61" s="1"/>
-      <c r="K61" s="2">
-        <v>2</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+        <v>149</v>
+      </c>
+      <c r="J61" s="5"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="2">
+        <v>2</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" s="2">
         <v>40</v>
       </c>
@@ -3369,10 +3517,10 @@
         <v>39</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="2">
@@ -3385,17 +3533,20 @@
         <v>36</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="J62" s="1"/>
-      <c r="K62" s="2">
+        <v>150</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="K62" s="1"/>
+      <c r="L62" s="2">
         <v>3</v>
       </c>
-      <c r="L62" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" s="2">
         <v>41</v>
       </c>
@@ -3403,10 +3554,10 @@
         <v>78</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="2">
@@ -3419,17 +3570,20 @@
         <v>36</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J63" s="1"/>
-      <c r="K63" s="2">
+        <v>151</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" s="2">
         <v>4</v>
       </c>
-      <c r="L63" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M63" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" s="2">
         <v>42</v>
       </c>
@@ -3437,10 +3591,10 @@
         <v>79</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="2">
@@ -3453,19 +3607,20 @@
         <v>36</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="K64" s="2">
-        <v>2</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
+        <v>152</v>
+      </c>
+      <c r="J64" s="5"/>
+      <c r="K64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L64" s="2">
+        <v>2</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" s="2">
         <v>43</v>
       </c>
@@ -3474,7 +3629,7 @@
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="2">
@@ -3487,17 +3642,18 @@
         <v>36</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="J65" s="1"/>
-      <c r="K65" s="2">
+        <v>153</v>
+      </c>
+      <c r="J65" s="5"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="2">
         <v>3</v>
       </c>
-      <c r="L65" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" s="23" customFormat="1">
+      <c r="M65" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="20">
         <v>44</v>
       </c>
@@ -3505,10 +3661,10 @@
         <v>81</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E66" s="21"/>
       <c r="F66" s="20">
@@ -3521,17 +3677,18 @@
         <v>36</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="J66" s="21"/>
-      <c r="K66" s="20">
-        <v>1</v>
-      </c>
-      <c r="L66" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" s="23" customFormat="1">
+        <v>177</v>
+      </c>
+      <c r="J66" s="22"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="20">
+        <v>1</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="20">
         <v>45</v>
       </c>
@@ -3539,10 +3696,10 @@
         <v>40</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E67" s="21"/>
       <c r="F67" s="20">
@@ -3555,17 +3712,18 @@
         <v>36</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="J67" s="21"/>
-      <c r="K67" s="20">
-        <v>2</v>
-      </c>
-      <c r="L67" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="23" customFormat="1">
+        <v>178</v>
+      </c>
+      <c r="J67" s="22"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="20">
+        <v>2</v>
+      </c>
+      <c r="M67" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" s="20">
         <v>46</v>
       </c>
@@ -3573,10 +3731,10 @@
         <v>41</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E68" s="21"/>
       <c r="F68" s="20">
@@ -3589,17 +3747,18 @@
         <v>36</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="J68" s="21"/>
-      <c r="K68" s="20">
+        <v>179</v>
+      </c>
+      <c r="J68" s="22"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="20">
         <v>3</v>
       </c>
-      <c r="L68" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="M68" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" s="2">
         <v>47</v>
       </c>
@@ -3607,10 +3766,10 @@
         <v>42</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="2">
@@ -3623,17 +3782,20 @@
         <v>36</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="J69" s="1"/>
-      <c r="K69" s="2">
+        <v>184</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="K69" s="1"/>
+      <c r="L69" s="2">
         <v>4</v>
       </c>
-      <c r="L69" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" s="2">
         <v>48</v>
       </c>
@@ -3642,7 +3804,7 @@
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="2"/>
@@ -3655,15 +3817,16 @@
       <c r="I70" s="5">
         <v>48</v>
       </c>
-      <c r="J70" s="1"/>
-      <c r="K70" s="2">
+      <c r="J70" s="5"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="2">
         <v>3</v>
       </c>
-      <c r="L70" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" s="2">
         <v>49</v>
       </c>
@@ -3671,10 +3834,10 @@
         <v>34</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="2">
@@ -3687,17 +3850,20 @@
         <v>48</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J71" s="1"/>
-      <c r="K71" s="2">
-        <v>1</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
+        <v>186</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="K71" s="1"/>
+      <c r="L71" s="2">
+        <v>1</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" s="2">
         <v>50</v>
       </c>
@@ -3705,10 +3871,10 @@
         <v>44</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="2">
@@ -3721,17 +3887,20 @@
         <v>48</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J72" s="1"/>
-      <c r="K72" s="2">
-        <v>2</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
+        <v>187</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="K72" s="1"/>
+      <c r="L72" s="2">
+        <v>2</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" s="2">
         <v>51</v>
       </c>
@@ -3739,10 +3908,10 @@
         <v>45</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="2">
@@ -3755,17 +3924,20 @@
         <v>48</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="J73" s="1"/>
-      <c r="K73" s="2">
+        <v>188</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="K73" s="1"/>
+      <c r="L73" s="2">
         <v>3</v>
       </c>
-      <c r="L73" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" s="2">
         <v>52</v>
       </c>
@@ -3773,10 +3945,10 @@
         <v>46</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="2">
@@ -3789,19 +3961,20 @@
         <v>48</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="K74" s="2">
+        <v>189</v>
+      </c>
+      <c r="J74" s="5"/>
+      <c r="K74" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="L74" s="2">
         <v>4</v>
       </c>
-      <c r="L74" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A75" s="2">
         <v>53</v>
       </c>
@@ -3809,10 +3982,10 @@
         <v>47</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="2">
@@ -3825,17 +3998,20 @@
         <v>48</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="J75" s="1"/>
-      <c r="K75" s="2">
+        <v>190</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="K75" s="1"/>
+      <c r="L75" s="2">
         <v>5</v>
       </c>
-      <c r="L75" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="M75" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A76" s="2">
         <v>54</v>
       </c>
@@ -3843,10 +4019,10 @@
         <v>48</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="2">
@@ -3859,17 +4035,20 @@
         <v>48</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="J76" s="1"/>
-      <c r="K76" s="2">
+        <v>191</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="K76" s="1"/>
+      <c r="L76" s="2">
         <v>6</v>
       </c>
-      <c r="L76" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A77" s="2">
         <v>55</v>
       </c>
@@ -3877,10 +4056,10 @@
         <v>51</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="2">
@@ -3893,17 +4072,20 @@
         <v>48</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="J77" s="1"/>
-      <c r="K77" s="2">
+        <v>192</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="K77" s="1"/>
+      <c r="L77" s="2">
         <v>7</v>
       </c>
-      <c r="L77" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="M77" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" s="2">
         <v>56</v>
       </c>
@@ -3911,10 +4093,10 @@
         <v>52</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="2">
@@ -3927,17 +4109,20 @@
         <v>48</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="J78" s="1"/>
-      <c r="K78" s="2">
+        <v>193</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="K78" s="1"/>
+      <c r="L78" s="2">
         <v>8</v>
       </c>
-      <c r="L78" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="M78" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A79" s="2">
         <v>57</v>
       </c>
@@ -3945,10 +4130,10 @@
         <v>53</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="2">
@@ -3961,17 +4146,20 @@
         <v>48</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="J79" s="1"/>
-      <c r="K79" s="2">
+        <v>194</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="K79" s="1"/>
+      <c r="L79" s="2">
         <v>9</v>
       </c>
-      <c r="L79" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A80" s="2">
         <v>58</v>
       </c>
@@ -3979,10 +4167,10 @@
         <v>35</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="2">
@@ -3995,26 +4183,29 @@
         <v>48</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="J80" s="1"/>
-      <c r="K80" s="2">
+        <v>195</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="K80" s="1"/>
+      <c r="L80" s="2">
         <v>10</v>
       </c>
-      <c r="L80" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A81" s="2">
         <v>59</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="2"/>
@@ -4027,15 +4218,16 @@
       <c r="I81" s="5">
         <v>59</v>
       </c>
-      <c r="J81" s="1"/>
-      <c r="K81" s="2">
+      <c r="J81" s="5"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="2">
         <v>4</v>
       </c>
-      <c r="L81" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="M81" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" s="2">
         <v>60</v>
       </c>
@@ -4043,10 +4235,10 @@
         <v>54</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="2">
@@ -4059,19 +4251,20 @@
         <v>59</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="J82" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="K82" s="2">
-        <v>1</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12">
+        <v>207</v>
+      </c>
+      <c r="J82" s="5"/>
+      <c r="K82" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="L82" s="2">
+        <v>1</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" s="2">
         <v>61</v>
       </c>
@@ -4079,10 +4272,10 @@
         <v>55</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="2">
@@ -4095,19 +4288,20 @@
         <v>59</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="K83" s="2">
-        <v>2</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12">
+        <v>208</v>
+      </c>
+      <c r="J83" s="5"/>
+      <c r="K83" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L83" s="2">
+        <v>2</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A84" s="2">
         <v>62</v>
       </c>
@@ -4115,10 +4309,10 @@
         <v>56</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="2">
@@ -4131,19 +4325,20 @@
         <v>59</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="K84" s="2">
+        <v>209</v>
+      </c>
+      <c r="J84" s="5"/>
+      <c r="K84" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="L84" s="2">
         <v>3</v>
       </c>
-      <c r="L84" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A85" s="2">
         <v>63</v>
       </c>
@@ -4151,10 +4346,10 @@
         <v>57</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="2">
@@ -4167,19 +4362,20 @@
         <v>59</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="K85" s="2">
+        <v>210</v>
+      </c>
+      <c r="J85" s="5"/>
+      <c r="K85" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L85" s="2">
         <v>4</v>
       </c>
-      <c r="L85" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="M85" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A86" s="2">
         <v>64</v>
       </c>
@@ -4187,10 +4383,10 @@
         <v>58</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="2">
@@ -4203,19 +4399,20 @@
         <v>59</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K86" s="2">
+        <v>211</v>
+      </c>
+      <c r="J86" s="5"/>
+      <c r="K86" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L86" s="2">
         <v>5</v>
       </c>
-      <c r="L86" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="M86" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A87" s="2">
         <v>65</v>
       </c>
@@ -4223,10 +4420,10 @@
         <v>59</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="2">
@@ -4239,19 +4436,20 @@
         <v>59</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="K87" s="2">
+        <v>212</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L87" s="2">
         <v>6</v>
       </c>
-      <c r="L87" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="M87" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A88" s="2">
         <v>66</v>
       </c>
@@ -4259,10 +4457,10 @@
         <v>60</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="2">
@@ -4275,19 +4473,20 @@
         <v>59</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="J88" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="K88" s="2">
+        <v>213</v>
+      </c>
+      <c r="J88" s="5"/>
+      <c r="K88" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L88" s="2">
         <v>7</v>
       </c>
-      <c r="L88" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A89" s="2">
         <v>67</v>
       </c>
@@ -4295,10 +4494,10 @@
         <v>61</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="2">
@@ -4311,17 +4510,20 @@
         <v>59</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J89" s="1"/>
-      <c r="K89" s="2">
+        <v>214</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="K89" s="1"/>
+      <c r="L89" s="2">
         <v>8</v>
       </c>
-      <c r="L89" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="M89" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A90" s="2">
         <v>68</v>
       </c>
@@ -4329,10 +4531,10 @@
         <v>62</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="2">
@@ -4345,19 +4547,20 @@
         <v>59</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="J90" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="K90" s="2">
+        <v>215</v>
+      </c>
+      <c r="J90" s="5"/>
+      <c r="K90" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L90" s="2">
         <v>9</v>
       </c>
-      <c r="L90" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A91" s="2">
         <v>69</v>
       </c>
@@ -4366,7 +4569,7 @@
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="2">
@@ -4379,28 +4582,29 @@
         <v>59</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="J91" s="1"/>
-      <c r="K91" s="2">
+        <v>216</v>
+      </c>
+      <c r="J91" s="5"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="2">
         <v>10</v>
       </c>
-      <c r="L91" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="M91" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A92" s="2">
         <v>70</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="2">
@@ -4413,19 +4617,20 @@
         <v>59</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="K92" s="2">
-        <v>1</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12">
+        <v>232</v>
+      </c>
+      <c r="J92" s="5"/>
+      <c r="K92" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L92" s="2">
+        <v>1</v>
+      </c>
+      <c r="M92" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A93" s="2">
         <v>71</v>
       </c>
@@ -4433,10 +4638,10 @@
         <v>64</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="2">
@@ -4449,30 +4654,31 @@
         <v>59</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K93" s="2">
-        <v>2</v>
-      </c>
-      <c r="L93" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12">
+        <v>233</v>
+      </c>
+      <c r="J93" s="5"/>
+      <c r="K93" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L93" s="2">
+        <v>2</v>
+      </c>
+      <c r="M93" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A94" s="2">
         <v>72</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="2">
@@ -4485,17 +4691,18 @@
         <v>59</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="J94" s="1"/>
-      <c r="K94" s="2">
+        <v>234</v>
+      </c>
+      <c r="J94" s="5"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="2">
         <v>3</v>
       </c>
-      <c r="L94" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="M94" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A95" s="2">
         <v>73</v>
       </c>
@@ -4503,10 +4710,10 @@
         <v>65</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="2">
@@ -4519,19 +4726,20 @@
         <v>59</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="J95" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="K95" s="2">
+        <v>235</v>
+      </c>
+      <c r="J95" s="5"/>
+      <c r="K95" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L95" s="2">
         <v>11</v>
       </c>
-      <c r="L95" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="M95" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A96" s="2">
         <v>74</v>
       </c>
@@ -4539,10 +4747,10 @@
         <v>66</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="2">
@@ -4555,20 +4763,21 @@
         <v>59</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="J96" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="K96" s="2">
+        <v>236</v>
+      </c>
+      <c r="J96" s="5"/>
+      <c r="K96" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="L96" s="2">
         <v>12</v>
       </c>
-      <c r="L96" s="2" t="s">
+      <c r="M96" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L96" xr:uid="{F9F1065D-2337-4AD4-BE05-642580AA564F}"/>
+  <autoFilter ref="A1:M96" xr:uid="{F9F1065D-2337-4AD4-BE05-642580AA564F}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4579,253 +4788,253 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B83A2D2-56B5-463C-80A8-B1FFE2FEB4DA}">
   <dimension ref="B1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="46.875" customWidth="1"/>
+    <col min="2" max="2" width="46.8984375" customWidth="1"/>
     <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B1" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>278</v>
-      </c>
       <c r="D1" s="26" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B2" s="28" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="27" t="s">
+        <v>275</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B3" s="28"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="27"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B4" s="28"/>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="27"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B5" s="28"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="27"/>
       <c r="C5" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B6" s="28"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="27"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B7" s="28"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="27"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B8" s="28"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="27"/>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B9" s="28"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="27"/>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B10" s="28"/>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="27"/>
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B11" s="28"/>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="27"/>
       <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B12" s="28"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="27"/>
       <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B13" s="28"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="27"/>
       <c r="C13" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B14" s="28"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="27"/>
       <c r="C14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B15" s="28"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="27"/>
       <c r="C15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B16" s="28"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="27"/>
       <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="16.5" customHeight="1">
-      <c r="B17" s="28"/>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="27"/>
       <c r="C17" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="28"/>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B18" s="27"/>
       <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="28"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B19" s="27"/>
       <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="28"/>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B20" s="27"/>
       <c r="C20" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="28"/>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B21" s="27"/>
       <c r="C21" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="28"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B22" s="27"/>
       <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="28"/>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B23" s="27"/>
       <c r="C23" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="28"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B24" s="27"/>
       <c r="C24" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="28"/>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B25" s="27"/>
       <c r="C25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="28"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B26" s="27"/>
       <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>